<commit_message>
Added box plot, minor tidy up
</commit_message>
<xml_diff>
--- a/data/SABA_Tidy_Data.xlsx
+++ b/data/SABA_Tidy_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="26680" windowHeight="15420"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="25875" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,16 +13,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$121</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -84,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,23 +413,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K126"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I114" sqref="I114"/>
+      <selection pane="bottomLeft" activeCell="H167" sqref="H167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="19.33203125" style="1"/>
-    <col min="6" max="6" width="19.33203125" style="3"/>
-    <col min="7" max="16384" width="19.33203125" style="1"/>
+    <col min="1" max="1" width="19.28515625" style="2"/>
+    <col min="2" max="5" width="19.28515625" style="1"/>
+    <col min="6" max="6" width="19.28515625" style="3"/>
+    <col min="7" max="16384" width="19.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3216,28 +3212,1147 @@
         <v>17</v>
       </c>
     </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B122" s="1">
+        <v>4</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F122" s="3">
+        <v>24.247407438283748</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B123" s="1">
+        <v>4</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F123" s="3">
+        <v>25.336861711899246</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="124" spans="1:11">
+      <c r="A124" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B124" s="1">
+        <v>4</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F124" s="3">
+        <v>23.180361624673441</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
     </row>
     <row r="125" spans="1:11">
+      <c r="A125" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B125" s="1">
+        <v>4</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F125" s="3">
+        <v>39.216802067711342</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
     </row>
     <row r="126" spans="1:11">
+      <c r="A126" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B126" s="1">
+        <v>4</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F126" s="3">
+        <v>42.487474604185017</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
     </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B127" s="1">
+        <v>4</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F127" s="3">
+        <v>42.674579264620064</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B128" s="1">
+        <v>4</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F128" s="3">
+        <v>0</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B129" s="1">
+        <v>4</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" s="3">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B130" s="1">
+        <v>4</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" s="3">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B131" s="1">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F131" s="3">
+        <v>674.57018105967245</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B132" s="1">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F132" s="3">
+        <v>671.73972487647609</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F133" s="3">
+        <v>674.49032539096618</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B134" s="1">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F134" s="3">
+        <v>219.66220577867603</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B135" s="1">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F135" s="3">
+        <v>219.9883690591526</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B136" s="1">
+        <v>4</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F136" s="3">
+        <v>219.88250363961626</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F137" s="3">
+        <v>0</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B138" s="1">
+        <v>4</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F138" s="3">
+        <v>0</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B139" s="1">
+        <v>4</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F139" s="3">
+        <v>0</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B140" s="1">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F140" s="3">
+        <v>0</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B141" s="1">
+        <v>4</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F141" s="3">
+        <v>0</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B142" s="1">
+        <v>4</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F142" s="3">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B143" s="1">
+        <v>4</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F143" s="3">
+        <v>880.27308079958141</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B144" s="1">
+        <v>4</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F144" s="3">
+        <v>873.08304729795998</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B145" s="1">
+        <v>4</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F145" s="3">
+        <v>876.58877610706145</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B146" s="1">
+        <v>4</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F146" s="3">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B147" s="1">
+        <v>4</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F147" s="3">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B148" s="1">
+        <v>4</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F148" s="3">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B149" s="1">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F149" s="3">
+        <v>881.8906347401728</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B150" s="1">
+        <v>4</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F150" s="3">
+        <v>873.18703214921061</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B151" s="1">
+        <v>4</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" s="3">
+        <v>874.17257924273395</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B152" s="1">
+        <v>4</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" s="3">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B153" s="1">
+        <v>4</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="3">
+        <v>0</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B154" s="1">
+        <v>4</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F154" s="3">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B155" s="1">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" s="3">
+        <v>0</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B156" s="1">
+        <v>4</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="3">
+        <v>0</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B157" s="1">
+        <v>4</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="3">
+        <v>0</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B158" s="1">
+        <v>4</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="3">
+        <v>676.8661303447567</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B159" s="1">
+        <v>4</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="3">
+        <v>658.84206265600517</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B160" s="1">
+        <v>4</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" s="3">
+        <v>671.71419526775571</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F161" s="3">
+        <v>715.86794899898121</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B162" s="1">
+        <v>4</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F162" s="3">
+        <v>696.98210430082668</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B163" s="1">
+        <v>4</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F163" s="3">
+        <v>643.01444418544997</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B164" s="1">
+        <v>5</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" s="3">
+        <v>39.811373785553158</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B165" s="1">
+        <v>5</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" s="3">
+        <v>39.231587363828758</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B166" s="1">
+        <v>5</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" s="3">
+        <v>39.613545858606031</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B167" s="1">
+        <v>5</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" s="3">
+        <v>41.804485214506315</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B168" s="1">
+        <v>5</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F168" s="3">
+        <v>216.9054970122526</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B169" s="1">
+        <v>5</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" s="3">
+        <v>215.2228876933541</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B170" s="1">
+        <v>5</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" s="3">
+        <v>215.63993317274861</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G121"/>
+  <autoFilter ref="A1:G121">
+    <filterColumn colId="2"/>
+    <filterColumn colId="5"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Trial 6 Data
</commit_message>
<xml_diff>
--- a/data/SABA_Tidy_Data.xlsx
+++ b/data/SABA_Tidy_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="25875" windowHeight="12330"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="25880" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$121</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -75,15 +80,43 @@
   <si>
     <t>Suspect</t>
   </si>
+  <si>
+    <t>CHEESE</t>
+  </si>
+  <si>
+    <t>TOPPING</t>
+  </si>
+  <si>
+    <t>TORTILLA</t>
+  </si>
+  <si>
+    <t>SPREAD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,8 +139,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -121,7 +156,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,20 +450,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K170"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H167" sqref="H167"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H203" sqref="H203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="2"/>
-    <col min="2" max="5" width="19.28515625" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="3"/>
-    <col min="7" max="16384" width="19.28515625" style="1"/>
+    <col min="1" max="1" width="19.33203125" style="2"/>
+    <col min="2" max="5" width="19.33203125" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="3"/>
+    <col min="7" max="16384" width="19.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4348,11 +4385,750 @@
         <v>17</v>
       </c>
     </row>
+    <row r="171" spans="1:7">
+      <c r="A171" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B171" s="1">
+        <v>6</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F171" s="3">
+        <v>23.060965224900105</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B172" s="1">
+        <v>6</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F172" s="3">
+        <v>22.609655800358333</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B173" s="1">
+        <v>6</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" s="3">
+        <v>21.962716702673763</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B174" s="1">
+        <v>6</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F174" s="3">
+        <v>0</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B175" s="1">
+        <v>6</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F175" s="3">
+        <v>0</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B176" s="1">
+        <v>6</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F176" s="3">
+        <v>0</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B177" s="1">
+        <v>6</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" s="3">
+        <v>652.82174998804385</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B178" s="1">
+        <v>6</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F178" s="3">
+        <v>663.49549014748868</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B179" s="1">
+        <v>6</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="3">
+        <v>651.01706713058377</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B180" s="1">
+        <v>6</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F180" s="3">
+        <v>0</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B181" s="1">
+        <v>6</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F181" s="3">
+        <v>0</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B182" s="1">
+        <v>6</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" s="3">
+        <v>0</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B183" s="1">
+        <v>6</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F183" s="3">
+        <v>0</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B184" s="1">
+        <v>6</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F184" s="3">
+        <v>0</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B185" s="1">
+        <v>6</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F185" s="3">
+        <v>0</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B186" s="1">
+        <v>6</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F186" s="3">
+        <v>0</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B187" s="1">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F187" s="3">
+        <v>854.47051958070517</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B188" s="1">
+        <v>6</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F188" s="3">
+        <v>876.7188382442896</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B189" s="1">
+        <v>6</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F189" s="3">
+        <v>867.06196980241714</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
+      <c r="A190" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B190" s="1">
+        <v>6</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F190" s="3">
+        <v>874.43857683344061</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
+      <c r="A191" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B191" s="1">
+        <v>6</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F191" s="3">
+        <v>878.35162173622086</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7">
+      <c r="A192" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B192" s="1">
+        <v>6</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F192" s="3">
+        <v>870.77361712123911</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B193" s="1">
+        <v>6</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F193" s="3">
+        <v>0</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7">
+      <c r="A194" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B194" s="1">
+        <v>6</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F194" s="3">
+        <v>0</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
+      <c r="A195" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B195" s="1">
+        <v>6</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F195" s="3">
+        <v>0</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B196" s="1">
+        <v>6</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F196" s="3">
+        <v>683.16861468096931</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B197" s="1">
+        <v>6</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F197" s="3">
+        <v>652.00532348705804</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B198" s="1">
+        <v>6</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F198" s="3">
+        <v>683.99401301188493</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B199" s="1">
+        <v>6</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F199" s="3">
+        <v>687.52511439963598</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B200" s="1">
+        <v>6</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F200" s="3">
+        <v>698.51206700455725</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B201" s="1">
+        <v>6</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F201" s="3">
+        <v>738.17933170909816</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B202" s="1">
+        <v>6</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F202" s="3">
+        <v>708.62944810280362</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G121">
-    <filterColumn colId="2"/>
-    <filterColumn colId="5"/>
-  </autoFilter>
+  <autoFilter ref="A1:G121"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>